<commit_message>
Added sum and max logs for Paillier, EC ElGamal, ORE, OPE
</commit_message>
<xml_diff>
--- a/analysis/S3 vs TreeDB Whole Range Sum.xlsx
+++ b/analysis/S3 vs TreeDB Whole Range Sum.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -3878,17 +3878,10 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>Inserted chunks</a:t>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t>Chunks number (N)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                  <a:t> count </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1400"/>
-                  <a:t>(N)</a:t>
-                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5030,8 +5023,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{409BC777-BE88-B440-B989-83CFADD528E0}">
   <dimension ref="A1:O601"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="W31" sqref="W31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>